<commit_message>
specification of the test
</commit_message>
<xml_diff>
--- a/prueba_dataanalyst.xlsx
+++ b/prueba_dataanalyst.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\william.uyasan\Documents\personal\prueba_dataanalyst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE5292B-DE7A-4236-BB63-DE6D52D86B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F90441-E530-4082-A0AE-EFB00715A4E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="2840" windowWidth="14400" windowHeight="7360" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parametros" sheetId="1" r:id="rId1"/>
@@ -2434,6 +2434,174 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="10"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="11"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -6001,6 +6169,126 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000001000000}" name="TablaDinámica27" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+  <location ref="N1:R8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Suma de pp_unidades_vendidas" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="3">
+    <chartFormat chart="9" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="9" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="9" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="TablaDinámica26" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
   <location ref="H1:L8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
@@ -6103,126 +6391,6 @@
           </reference>
           <reference field="1" count="1" selected="0">
             <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000001000000}" name="TablaDinámica27" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
-  <location ref="N1:R8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="6">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Suma de pp_unidades_vendidas" fld="4" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="3">
-    <chartFormat chart="9" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="9" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="9" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
           </reference>
         </references>
       </pivotArea>
@@ -8507,8 +8675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C6"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>